<commit_message>
fix upload excel admin
</commit_message>
<xml_diff>
--- a/questionnaires (2).xlsx
+++ b/questionnaires (2).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\projectrumah\frontendnew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8273D06-C421-4078-B48D-9652D1656F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D186864-4D96-4D87-ADAF-8697D1CD21BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questionnaires" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="130">
   <si>
     <t>nomorUrut</t>
   </si>
@@ -208,15 +208,9 @@
     <t>Bukit Damai</t>
   </si>
   <si>
-    <t>S2</t>
-  </si>
-  <si>
     <t>Karyawan Swasta</t>
   </si>
   <si>
-    <t>Rumah Tinggal/Hunian</t>
-  </si>
-  <si>
     <t>Milik Sendiri</t>
   </si>
   <si>
@@ -226,15 +220,9 @@
     <t>Tidak Ada</t>
   </si>
   <si>
-    <t>Listrik Non PLN</t>
-  </si>
-  <si>
     <t>1300</t>
   </si>
   <si>
-    <t>Pernah, &lt;10 Tahun</t>
-  </si>
-  <si>
     <t>Semi Permanen</t>
   </si>
   <si>
@@ -247,33 +235,15 @@
     <t>Tanah</t>
   </si>
   <si>
-    <t>Spandek</t>
-  </si>
-  <si>
     <t>Asbes</t>
   </si>
   <si>
     <t>Jaringan Perpipaan</t>
   </si>
   <si>
-    <t>Tidak Tersedia</t>
-  </si>
-  <si>
     <t>Terpelihara</t>
   </si>
   <si>
-    <t>Pantai/Tanah Lapangan/Kebun</t>
-  </si>
-  <si>
-    <t>Bersama/MCK Komunal</t>
-  </si>
-  <si>
-    <t>Leher Angsa</t>
-  </si>
-  <si>
-    <t>Pabrikasi</t>
-  </si>
-  <si>
     <t>Batu Bata</t>
   </si>
   <si>
@@ -286,9 +256,6 @@
     <t>PDAM</t>
   </si>
   <si>
-    <t>-6.200000,106.816666</t>
-  </si>
-  <si>
     <t>2024-11-05</t>
   </si>
   <si>
@@ -440,6 +407,9 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Tidak Berpenghuni</t>
   </si>
 </sst>
 </file>
@@ -819,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="BH5" sqref="BH5"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -890,13 +860,13 @@
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1067,12 +1037,12 @@
         <v>56</v>
       </c>
       <c r="BH1" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1081,28 +1051,28 @@
         <v>123</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="E2">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>57</v>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
       </c>
       <c r="G2" s="1">
-        <v>1234567891011230</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1">
-        <v>1234567891011230</v>
-      </c>
-      <c r="I2" t="s">
-        <v>58</v>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L2" t="s">
         <v>59</v>
@@ -1113,137 +1083,137 @@
       <c r="N2" t="s">
         <v>61</v>
       </c>
-      <c r="O2" t="s">
-        <v>62</v>
-      </c>
-      <c r="P2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>64</v>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>900000</v>
-      </c>
-      <c r="S2" t="s">
-        <v>65</v>
-      </c>
-      <c r="T2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U2" t="s">
-        <v>65</v>
-      </c>
-      <c r="V2" t="s">
-        <v>67</v>
-      </c>
-      <c r="W2" t="s">
-        <v>68</v>
-      </c>
-      <c r="X2" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>73</v>
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
       </c>
       <c r="AO2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AP2">
-        <v>120</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AR2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BC2">
+        <v>0</v>
+      </c>
+      <c r="BD2">
+        <v>0</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BG2" t="s">
         <v>78</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AV2">
-        <v>2</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>85</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>86</v>
-      </c>
-      <c r="BC2">
-        <v>9</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>88</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>89</v>
       </c>
       <c r="BH2">
         <v>11</v>
@@ -1251,7 +1221,7 @@
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1260,7 +1230,7 @@
         <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="E3">
         <v>35</v>
@@ -1287,88 +1257,88 @@
         <v>59</v>
       </c>
       <c r="M3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="N3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="O3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="P3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q3" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="R3">
         <v>10000000</v>
       </c>
       <c r="S3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T3" t="s">
+        <v>64</v>
+      </c>
+      <c r="U3" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" t="s">
+        <v>64</v>
+      </c>
+      <c r="W3" t="s">
+        <v>83</v>
+      </c>
+      <c r="X3" t="s">
         <v>66</v>
       </c>
-      <c r="U3" t="s">
-        <v>65</v>
-      </c>
-      <c r="V3" t="s">
-        <v>66</v>
-      </c>
-      <c r="W3" t="s">
-        <v>94</v>
-      </c>
-      <c r="X3" t="s">
-        <v>69</v>
-      </c>
       <c r="Y3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="Z3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="AA3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="AB3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="AC3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="AD3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="AE3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="AF3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="AG3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="AH3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AI3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="AJ3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="AK3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="AL3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="AM3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="AN3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="AO3">
         <v>100</v>
@@ -1377,52 +1347,52 @@
         <v>120</v>
       </c>
       <c r="AQ3" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="AR3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="AS3" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="AT3" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="AU3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AV3">
         <v>2</v>
       </c>
       <c r="AW3" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="AX3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="AY3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="AZ3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="BA3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="BB3" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="BC3">
         <v>10</v>
       </c>
       <c r="BD3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="BF3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="BG3" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="BH3">
         <v>11</v>
@@ -1430,7 +1400,7 @@
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1439,7 +1409,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E4">
         <v>14</v>
@@ -1448,10 +1418,10 @@
         <v>57</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="H4" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="I4" t="s">
         <v>58</v>
@@ -1463,91 +1433,91 @@
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="M4" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="N4" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="O4" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="P4" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="Q4" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="R4">
         <v>4300000</v>
       </c>
       <c r="S4" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="T4" t="s">
+        <v>65</v>
+      </c>
+      <c r="U4" t="s">
+        <v>107</v>
+      </c>
+      <c r="V4" t="s">
+        <v>65</v>
+      </c>
+      <c r="W4" t="s">
+        <v>108</v>
+      </c>
+      <c r="X4" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z4" t="s">
         <v>67</v>
       </c>
-      <c r="U4" t="s">
-        <v>118</v>
-      </c>
-      <c r="V4" t="s">
-        <v>67</v>
-      </c>
-      <c r="W4" t="s">
-        <v>119</v>
-      </c>
-      <c r="X4" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM4" t="s">
         <v>71</v>
       </c>
-      <c r="AA4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>122</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>123</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>76</v>
-      </c>
       <c r="AN4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AO4">
         <v>100</v>
@@ -1556,55 +1526,55 @@
         <v>132</v>
       </c>
       <c r="AQ4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AR4" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="AS4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="AT4" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="AU4" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="AV4">
         <v>1</v>
       </c>
       <c r="AW4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="AX4" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="AY4" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="AZ4" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="BA4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="BB4" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="BC4">
         <v>9</v>
       </c>
       <c r="BD4" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="BE4" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="BF4" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="BG4" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="BH4">
         <v>11</v>
@@ -1612,6 +1582,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upload update excel modal search
</commit_message>
<xml_diff>
--- a/questionnaires (2).xlsx
+++ b/questionnaires (2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\projectrumah\frontendnew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D186864-4D96-4D87-ADAF-8697D1CD21BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D58A13-AD88-4BAA-90FE-74C519C4D5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3936" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questionnaires" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="130">
   <si>
     <t>nomorUrut</t>
   </si>
@@ -199,9 +199,6 @@
     <t>KSB</t>
   </si>
   <si>
-    <t>Jl. Kebon Jeruk No. 10</t>
-  </si>
-  <si>
     <t>Maluk</t>
   </si>
   <si>
@@ -259,9 +256,6 @@
     <t>2024-11-05</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Kebon Jeruk</t>
   </si>
   <si>
@@ -410,6 +404,12 @@
   </si>
   <si>
     <t>Tidak Berpenghuni</t>
+  </si>
+  <si>
+    <t>test firut upload update</t>
+  </si>
+  <si>
+    <t>update</t>
   </si>
 </sst>
 </file>
@@ -787,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH4"/>
+  <dimension ref="A1:BH5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -860,13 +860,13 @@
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1037,12 +1037,12 @@
         <v>56</v>
       </c>
       <c r="BH1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1051,7 +1051,7 @@
         <v>123</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1075,14 +1075,14 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M2" t="s">
         <v>59</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>60</v>
       </c>
-      <c r="N2" t="s">
-        <v>61</v>
-      </c>
       <c r="O2">
         <v>0</v>
       </c>
@@ -1213,15 +1213,15 @@
         <v>0</v>
       </c>
       <c r="BG2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="BH2">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1230,7 +1230,7 @@
         <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E3">
         <v>35</v>
@@ -1254,91 +1254,91 @@
         <v>4</v>
       </c>
       <c r="L3" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
       <c r="M3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O3" t="s">
+        <v>79</v>
+      </c>
+      <c r="P3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q3" t="s">
         <v>80</v>
-      </c>
-      <c r="N3" t="s">
-        <v>80</v>
-      </c>
-      <c r="O3" t="s">
-        <v>81</v>
-      </c>
-      <c r="P3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>82</v>
       </c>
       <c r="R3">
         <v>10000000</v>
       </c>
       <c r="S3" t="s">
+        <v>62</v>
+      </c>
+      <c r="T3" t="s">
         <v>63</v>
       </c>
-      <c r="T3" t="s">
-        <v>64</v>
-      </c>
       <c r="U3" t="s">
+        <v>62</v>
+      </c>
+      <c r="V3" t="s">
         <v>63</v>
       </c>
-      <c r="V3" t="s">
-        <v>64</v>
-      </c>
       <c r="W3" t="s">
+        <v>81</v>
+      </c>
+      <c r="X3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z3" t="s">
         <v>83</v>
       </c>
-      <c r="X3" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>84</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC3" t="s">
         <v>85</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AD3" t="s">
         <v>86</v>
       </c>
-      <c r="AB3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC3" t="s">
+      <c r="AE3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG3" t="s">
         <v>87</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AH3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI3" t="s">
         <v>88</v>
       </c>
-      <c r="AE3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AG3" t="s">
+      <c r="AJ3" t="s">
         <v>89</v>
       </c>
-      <c r="AH3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI3" t="s">
+      <c r="AK3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM3" t="s">
         <v>90</v>
       </c>
-      <c r="AJ3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>92</v>
-      </c>
       <c r="AN3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AO3">
         <v>100</v>
@@ -1347,60 +1347,60 @@
         <v>120</v>
       </c>
       <c r="AQ3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS3" t="s">
         <v>93</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="AT3" t="s">
         <v>94</v>
       </c>
-      <c r="AS3" t="s">
-        <v>95</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>96</v>
-      </c>
       <c r="AU3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AV3">
         <v>2</v>
       </c>
       <c r="AW3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AX3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AY3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AZ3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BA3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BB3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="BC3">
         <v>10</v>
       </c>
       <c r="BD3" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>97</v>
+      </c>
+      <c r="BG3" t="s">
         <v>77</v>
       </c>
-      <c r="BF3" t="s">
-        <v>99</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>78</v>
-      </c>
       <c r="BH3">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1409,7 +1409,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E4">
         <v>14</v>
@@ -1418,10 +1418,10 @@
         <v>57</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I4" t="s">
         <v>58</v>
@@ -1433,91 +1433,91 @@
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>79</v>
+        <v>129</v>
       </c>
       <c r="M4" t="s">
+        <v>99</v>
+      </c>
+      <c r="N4" t="s">
+        <v>100</v>
+      </c>
+      <c r="O4" t="s">
         <v>101</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>102</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>103</v>
-      </c>
-      <c r="P4" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>105</v>
       </c>
       <c r="R4">
         <v>4300000</v>
       </c>
       <c r="S4" t="s">
+        <v>104</v>
+      </c>
+      <c r="T4" t="s">
+        <v>64</v>
+      </c>
+      <c r="U4" t="s">
+        <v>105</v>
+      </c>
+      <c r="V4" t="s">
+        <v>64</v>
+      </c>
+      <c r="W4" t="s">
         <v>106</v>
       </c>
-      <c r="T4" t="s">
-        <v>65</v>
-      </c>
-      <c r="U4" t="s">
+      <c r="X4" t="s">
         <v>107</v>
       </c>
-      <c r="V4" t="s">
-        <v>65</v>
-      </c>
-      <c r="W4" t="s">
+      <c r="Y4" t="s">
         <v>108</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Z4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI4" t="s">
         <v>109</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AJ4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK4" t="s">
         <v>110</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AL4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN4" t="s">
         <v>67</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>112</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>68</v>
       </c>
       <c r="AO4">
         <v>100</v>
@@ -1526,58 +1526,240 @@
         <v>132</v>
       </c>
       <c r="AQ4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AS4" t="s">
         <v>72</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AT4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AU4" t="s">
         <v>113</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>114</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>115</v>
       </c>
       <c r="AV4">
         <v>1</v>
       </c>
       <c r="AW4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AY4" t="s">
         <v>116</v>
       </c>
-      <c r="AX4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>118</v>
-      </c>
       <c r="AZ4" t="s">
+        <v>74</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BB4" t="s">
         <v>75</v>
-      </c>
-      <c r="BA4" t="s">
-        <v>64</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>76</v>
       </c>
       <c r="BC4">
         <v>9</v>
       </c>
       <c r="BD4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BE4" t="s">
+        <v>117</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>118</v>
+      </c>
+      <c r="BG4" t="s">
         <v>119</v>
       </c>
-      <c r="BF4" t="s">
-        <v>120</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>121</v>
-      </c>
       <c r="BH4">
-        <v>11</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>129</v>
+      </c>
+      <c r="M5" t="s">
+        <v>99</v>
+      </c>
+      <c r="N5" t="s">
+        <v>100</v>
+      </c>
+      <c r="O5" t="s">
+        <v>101</v>
+      </c>
+      <c r="P5" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>103</v>
+      </c>
+      <c r="R5">
+        <v>4300000</v>
+      </c>
+      <c r="S5" t="s">
+        <v>104</v>
+      </c>
+      <c r="T5" t="s">
+        <v>64</v>
+      </c>
+      <c r="U5" t="s">
+        <v>105</v>
+      </c>
+      <c r="V5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W5" t="s">
+        <v>106</v>
+      </c>
+      <c r="X5" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO5">
+        <v>100</v>
+      </c>
+      <c r="AP5">
+        <v>132</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>111</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AV5">
+        <v>1</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>114</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>115</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>74</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>63</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC5">
+        <v>9</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>117</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>118</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>119</v>
+      </c>
+      <c r="BH5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>